<commit_message>
Adds some Actuators, updates sensors, adds Stories, finishes the Widora air pinout.
</commit_message>
<xml_diff>
--- a/docs/pinouts/Widora air/Widora air.xlsx
+++ b/docs/pinouts/Widora air/Widora air.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AECCA5-7131-4896-B194-CBC738483351}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446FBE6A-027B-4355-8CFD-345F22C3EF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{E2CC1134-D58F-4113-84C8-9B22D579265A}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>TOUCH</t>
   </si>
@@ -163,17 +163,20 @@
     <t>https://github.com/espruino/Espruino/issues/1574</t>
   </si>
   <si>
-    <t>The IC2 interface</t>
-  </si>
-  <si>
-    <t>The SPI interface</t>
+    <t>The IC2 interface used by some components. Example: BMP180 Atmospheric Pressure Sensor</t>
+  </si>
+  <si>
+    <t>The SPI interface used by some components. Example: DS3231 RTC Module</t>
+  </si>
+  <si>
+    <t>Not sure if it works in Espruino: http://forum.espruino.com/conversations/328396/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +210,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,9 +670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C69D95E-040B-4473-A5C7-366E8E934A18}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -725,10 +741,10 @@
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -739,10 +755,10 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -772,10 +788,10 @@
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="J4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -827,8 +843,8 @@
       <c r="I5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="2" t="s">
         <v>0</v>
       </c>
@@ -872,10 +888,10 @@
       <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -1281,32 +1297,59 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{FFFB3DD6-7F24-48A9-A032-73A0473597D6}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{FFFB3DD6-7F24-48A9-A032-73A0473597D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Finishes the Widora air pinout.
</commit_message>
<xml_diff>
--- a/docs/pinouts/Widora air/Widora air.xlsx
+++ b/docs/pinouts/Widora air/Widora air.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6908D3B5-6080-4842-85D5-B49A2A4FDEB1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0BEBBF-085F-4A26-B157-AB3756A3A3B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{E2CC1134-D58F-4113-84C8-9B22D579265A}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
   <si>
     <t>TOUCH</t>
   </si>
@@ -130,12 +130,6 @@
     <t>D17</t>
   </si>
   <si>
-    <t>Espruino pin code:</t>
-  </si>
-  <si>
-    <t>Do not work on Espruino</t>
-  </si>
-  <si>
     <t>Usage:</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>Features:</t>
   </si>
   <si>
-    <t>Input only</t>
-  </si>
-  <si>
     <t>Input and output. Example usage: turn a relay on or off (digitalWrite), verify the state of a switch (digitalRead).</t>
   </si>
   <si>
@@ -163,20 +154,47 @@
     <t>https://github.com/espruino/Espruino/issues/1574</t>
   </si>
   <si>
-    <t>The IC2 interface used by some components. Example: BMP180 Atmospheric Pressure Sensor</t>
-  </si>
-  <si>
     <t>The SPI interface used by some components. Example: DS3231 RTC Module</t>
   </si>
   <si>
     <t>Capacitive touch. Not sure if it works in Espruino: http://forum.espruino.com/conversations/328396/</t>
+  </si>
+  <si>
+    <t>5V*</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>on Espruino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not work </t>
+  </si>
+  <si>
+    <t>Directly connected to the USB input voltage. Can be used to power 5V sensors/actuators or to provide power to the board.</t>
+  </si>
+  <si>
+    <t>Espruino pin:</t>
+  </si>
+  <si>
+    <t>Espruino pin</t>
+  </si>
+  <si>
+    <t>Input only.</t>
+  </si>
+  <si>
+    <t>The IC2 interface used by some components. Example: BMP180 Atmospheric Pressure Sensor.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +240,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -249,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -266,12 +300,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,14 +417,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -349,8 +514,8 @@
       <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>264780</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>351371</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>4780483</xdr:rowOff>
     </xdr:to>
@@ -375,7 +540,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="606136" y="2078182"/>
+          <a:off x="0" y="2078182"/>
           <a:ext cx="17271235" cy="4763165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -688,354 +853,374 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="10.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="I1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="J1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="22"/>
       <c r="U1" s="13"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="13"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="15" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="M3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="33"/>
       <c r="U3" s="13"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="33" t="s">
+        <v>1</v>
+      </c>
       <c r="U4" s="13"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="E5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="F5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="H5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="I5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="J5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="K5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="O5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
       <c r="U5" s="13"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="13"/>
       <c r="Q6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="K7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="L7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="N7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="O7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="P7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="Q7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13" t="s">
+      <c r="R7" s="13"/>
+      <c r="S7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="T7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
       <c r="U7" s="13"/>
-    </row>
-    <row r="8" spans="1:21" ht="384" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+    </row>
+    <row r="8" spans="1:23" ht="377.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1054,226 +1239,256 @@
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="N9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="O9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="P9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="Q9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="R9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="13" t="s">
+      <c r="S9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="T9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
       <c r="U9" s="13"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="R11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="T11" s="22" t="s">
+        <v>3</v>
+      </c>
       <c r="U11" s="13"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="N12" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="O12" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="P12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="Q12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="16" t="s">
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
       <c r="U12" s="13"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="30"/>
       <c r="U13" s="13"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1281,7 +1496,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1289,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1297,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1305,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1313,23 +1528,28 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" xr:uid="{FFFB3DD6-7F24-48A9-A032-73A0473597D6}"/>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{FFFB3DD6-7F24-48A9-A032-73A0473597D6}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>